<commit_message>
error resolved and vertiport and pads name changed
</commit_message>
<xml_diff>
--- a/vertiport_info_144_12.xlsx
+++ b/vertiport_info_144_12.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Thesis\run_files_1402_02_27_20\capacity_distance_20_capcaity_4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thesis\Projects\simple_airport\thesis\UAM_network\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20839C8B-97F2-4FA6-A1E7-B984DA620763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33863B6C-544B-418B-8151-9099C636868E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -36,15 +36,6 @@
     <t>[0,0]</t>
   </si>
   <si>
-    <t>Airport 1</t>
-  </si>
-  <si>
-    <t>PositionStart</t>
-  </si>
-  <si>
-    <t>Airport 2</t>
-  </si>
-  <si>
     <t>AircraftID</t>
   </si>
   <si>
@@ -54,58 +45,58 @@
     <t>Pad</t>
   </si>
   <si>
-    <t>Airport1_Pad1</t>
-  </si>
-  <si>
-    <t>Airport1_Pad2</t>
-  </si>
-  <si>
-    <t>Airport1_Pad3</t>
-  </si>
-  <si>
-    <t>Airport1_Pad4</t>
-  </si>
-  <si>
-    <t>Airport2_Pad1</t>
-  </si>
-  <si>
-    <t>Airport2_Pad2</t>
-  </si>
-  <si>
-    <t>Airport2_Pad3</t>
-  </si>
-  <si>
-    <t>Airport2_Pad4</t>
-  </si>
-  <si>
-    <t>Airport3_Pad1</t>
-  </si>
-  <si>
-    <t>Airport3_Pad2</t>
-  </si>
-  <si>
-    <t>Airport3_Pad3</t>
-  </si>
-  <si>
-    <t>Airport3_Pad4</t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
-    <t>PadDirection</t>
-  </si>
-  <si>
-    <t>PadLength</t>
-  </si>
-  <si>
-    <t>PadWidth</t>
-  </si>
-  <si>
     <t>[10,17.32]</t>
   </si>
   <si>
     <t>[-10,17.32]</t>
+  </si>
+  <si>
+    <t>Vertiport1_Pad1</t>
+  </si>
+  <si>
+    <t>Vertiport1_Pad2</t>
+  </si>
+  <si>
+    <t>Vertiport1_Pad3</t>
+  </si>
+  <si>
+    <t>Vertiport1_Pad4</t>
+  </si>
+  <si>
+    <t>Vertiport2_Pad1</t>
+  </si>
+  <si>
+    <t>Vertiport2_Pad2</t>
+  </si>
+  <si>
+    <t>Vertiport2_Pad3</t>
+  </si>
+  <si>
+    <t>Vertiport2_Pad4</t>
+  </si>
+  <si>
+    <t>Vertiport3_Pad1</t>
+  </si>
+  <si>
+    <t>Vertiport3_Pad2</t>
+  </si>
+  <si>
+    <t>Vertiport3_Pad3</t>
+  </si>
+  <si>
+    <t>Vertiport3_Pad4</t>
+  </si>
+  <si>
+    <t>Vertiport 1</t>
+  </si>
+  <si>
+    <t>Vertiport 2</t>
+  </si>
+  <si>
+    <t>Vertiport 3</t>
   </si>
 </sst>
 </file>
@@ -432,26 +423,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G13"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="2" width="8.88671875" style="1"/>
     <col min="3" max="3" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" style="1"/>
-    <col min="9" max="9" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="1"/>
+    <col min="4" max="4" width="8.88671875" style="1"/>
+    <col min="5" max="5" width="13.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,33 +446,21 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>24</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
@@ -494,242 +469,98 @@
         <v>9</v>
       </c>
       <c r="D2" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>12000</v>
+        <v>4</v>
       </c>
       <c r="F2" s="1">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2" s="1">
-        <v>1</v>
-      </c>
-      <c r="I2" s="1">
-        <v>4</v>
-      </c>
-      <c r="J2" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
-        <v>150</v>
-      </c>
-      <c r="E3" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F3" s="1">
-        <v>60</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="1">
-        <v>150</v>
-      </c>
-      <c r="E4" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F4" s="1">
-        <v>120</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D5" s="1">
-        <v>150</v>
-      </c>
-      <c r="E5" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F5" s="1">
-        <v>180</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>12000</v>
+        <v>4</v>
       </c>
       <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H6" s="1">
-        <v>1</v>
-      </c>
-      <c r="I6" s="1">
-        <v>4</v>
-      </c>
-      <c r="J6" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1">
-        <v>150</v>
-      </c>
-      <c r="E7" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F7" s="1">
-        <v>60</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="1">
-        <v>150</v>
-      </c>
-      <c r="E8" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F8" s="1">
-        <v>120</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="1">
-        <v>150</v>
-      </c>
-      <c r="E9" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F9" s="1">
-        <v>180</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>5</v>
+        <v>23</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="1">
-        <v>150</v>
+        <v>1</v>
       </c>
       <c r="E10" s="1">
-        <v>12000</v>
+        <v>4</v>
       </c>
       <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H10" s="1">
-        <v>1</v>
-      </c>
-      <c r="I10" s="1">
-        <v>4</v>
-      </c>
-      <c r="J10" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="1">
-        <v>150</v>
-      </c>
-      <c r="E11" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F11" s="1">
-        <v>60</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="1">
-        <v>150</v>
-      </c>
-      <c r="E12" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F12" s="1">
-        <v>120</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C13" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="D13" s="1">
-        <v>150</v>
-      </c>
-      <c r="E13" s="1">
-        <v>12000</v>
-      </c>
-      <c r="F13" s="1">
-        <v>180</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>